<commit_message>
Update Excel test data and fix batch file path issue
- Updated Simple Test Data.xlsx with latest test information
- Fixed update-tests.bat to handle directory paths correctly (removed trailing backslash)

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Results/Simple Test Data.xlsx
+++ b/Results/Simple Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VH Website\vh-website\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F13CE8B-209C-4BA2-87D0-299F89FD7213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F88173B-B7D5-4373-B916-DAD20A19BB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
@@ -359,7 +359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -386,6 +386,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3053,7 +3054,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3189,7 +3190,7 @@
       </c>
       <c r="L3">
         <f t="shared" ref="L3:L25" si="3">_xlfn.RANK.EQ(K3,$K$2:$K$25)</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M3">
         <v>12</v>
@@ -3234,7 +3235,7 @@
       </c>
       <c r="L4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M4">
         <v>12</v>
@@ -3279,7 +3280,7 @@
       </c>
       <c r="L5">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M5">
         <v>12</v>
@@ -3324,7 +3325,7 @@
       </c>
       <c r="L6">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M6">
         <v>12</v>
@@ -3369,7 +3370,7 @@
       </c>
       <c r="L7">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M7">
         <v>12</v>
@@ -3414,7 +3415,7 @@
       </c>
       <c r="L8">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M8">
         <v>12</v>
@@ -3428,7 +3429,7 @@
         <v>15</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -3438,7 +3439,7 @@
       </c>
       <c r="F9">
         <f t="shared" ref="F9" si="4">C9</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -3455,11 +3456,11 @@
       </c>
       <c r="K9">
         <f t="shared" ref="K9" si="6">F9+J9</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L9">
         <f t="shared" ref="L9" si="7">_xlfn.RANK.EQ(K9,$K$2:$K$25)</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M9">
         <v>12</v>
@@ -3504,7 +3505,7 @@
       </c>
       <c r="L10">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M10">
         <v>12</v>
@@ -3549,7 +3550,7 @@
       </c>
       <c r="L11">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M11">
         <v>12</v>
@@ -3594,7 +3595,7 @@
       </c>
       <c r="L12">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M12">
         <v>12</v>
@@ -3729,7 +3730,7 @@
       </c>
       <c r="L15">
         <f t="shared" si="3"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M15">
         <v>12</v>
@@ -3774,7 +3775,7 @@
       </c>
       <c r="L16">
         <f t="shared" si="3"/>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M16">
         <v>12</v>
@@ -3819,7 +3820,7 @@
       </c>
       <c r="L17">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M17">
         <v>12</v>
@@ -3833,7 +3834,7 @@
         <v>33</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -3843,10 +3844,10 @@
       </c>
       <c r="F18">
         <f t="shared" ref="F18" si="12">C18</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -3856,15 +3857,15 @@
       </c>
       <c r="J18">
         <f t="shared" ref="J18" si="13">G18</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="K18">
         <f t="shared" ref="K18" si="14">F18+J18</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="L18">
         <f t="shared" ref="L18" si="15">_xlfn.RANK.EQ(K18,$K$2:$K$25)</f>
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="M18">
         <v>12</v>
@@ -3909,7 +3910,7 @@
       </c>
       <c r="L19">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M19">
         <v>12</v>
@@ -3954,7 +3955,7 @@
       </c>
       <c r="L20">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M20">
         <v>12</v>
@@ -4044,7 +4045,7 @@
       </c>
       <c r="L22">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M22">
         <v>12</v>
@@ -4089,7 +4090,7 @@
       </c>
       <c r="L23">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M23">
         <v>12</v>
@@ -4134,7 +4135,7 @@
       </c>
       <c r="L24">
         <f t="shared" ref="L24" si="19">_xlfn.RANK.EQ(K24,$K$2:$K$25)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M24">
         <v>13</v>
@@ -4194,8 +4195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8377D7-87E1-4BD8-A212-2056BAB3845F}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4287,7 +4288,7 @@
       </c>
       <c r="L2">
         <f>_xlfn.RANK.EQ(K2,$K$2:$K$25)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M2">
         <v>12</v>
@@ -4301,18 +4302,18 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D25" si="0">E3-C3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F25" si="1">C3</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -4329,12 +4330,12 @@
         <v>2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K25" si="4">F3+J3</f>
-        <v>5</v>
+        <f>C3*2.5</f>
+        <v>10</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L25" si="5">_xlfn.RANK.EQ(K3,$K$2:$K$25)</f>
-        <v>10</v>
+        <f t="shared" ref="L3:L25" si="4">_xlfn.RANK.EQ(K3,$K$2:$K$25)</f>
+        <v>11</v>
       </c>
       <c r="M3">
         <v>12</v>
@@ -4348,18 +4349,18 @@
         <v>7</v>
       </c>
       <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
         <v>8</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="1"/>
-        <v>2</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -4376,12 +4377,12 @@
         <v>4</v>
       </c>
       <c r="K4">
+        <f>C4*2.5</f>
+        <v>20</v>
+      </c>
+      <c r="L4">
         <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="5"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M4">
         <v>12</v>
@@ -4423,12 +4424,12 @@
         <v>4</v>
       </c>
       <c r="K5">
+        <f t="shared" ref="K3:K25" si="5">F5+J5</f>
+        <v>6</v>
+      </c>
+      <c r="L5">
         <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="5"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="M5">
         <v>12</v>
@@ -4470,12 +4471,12 @@
         <v>8</v>
       </c>
       <c r="K6">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="L6">
         <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="M6">
         <v>12</v>
@@ -4514,12 +4515,12 @@
         <v>0</v>
       </c>
       <c r="K7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M7">
         <v>12</v>
@@ -4561,12 +4562,12 @@
         <v>7</v>
       </c>
       <c r="K8">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="M8">
         <v>12</v>
@@ -4576,40 +4577,44 @@
       <c r="A9">
         <v>400651</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
       <c r="G9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H9">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I9">
         <v>15</v>
       </c>
       <c r="J9">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K9">
+        <f>C9*2.5</f>
+        <v>15</v>
+      </c>
+      <c r="L9">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="5"/>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="M9">
         <v>12</v>
@@ -4648,12 +4653,12 @@
         <v>0</v>
       </c>
       <c r="K10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M10">
         <v>12</v>
@@ -4667,15 +4672,15 @@
         <v>19</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
@@ -4689,12 +4694,12 @@
         <v>0</v>
       </c>
       <c r="K11">
+        <f>C11*2.5</f>
+        <v>7.5</v>
+      </c>
+      <c r="L11">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M11">
         <v>12</v>
@@ -4733,12 +4738,12 @@
         <v>0</v>
       </c>
       <c r="K12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L12">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M12">
         <v>12</v>
@@ -4777,12 +4782,12 @@
         <v>0</v>
       </c>
       <c r="K13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L13">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M13">
         <v>12</v>
@@ -4792,44 +4797,44 @@
       <c r="A14">
         <v>196303</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C14">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>10</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G14">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I14">
         <v>15</v>
       </c>
       <c r="J14">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K14">
+        <f>C14*2.5</f>
+        <v>22.5</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M14">
         <v>12</v>
@@ -4868,12 +4873,12 @@
         <v>0</v>
       </c>
       <c r="K15">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L15">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M15">
         <v>12</v>
@@ -4912,12 +4917,12 @@
         <v>0</v>
       </c>
       <c r="K16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M16">
         <v>12</v>
@@ -4956,12 +4961,12 @@
         <v>0</v>
       </c>
       <c r="K17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M17">
         <v>12</v>
@@ -4971,19 +4976,19 @@
       <c r="A18">
         <v>643388</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="12" t="s">
         <v>33</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H18">
         <f t="shared" si="2"/>
@@ -4997,12 +5002,12 @@
         <v>0</v>
       </c>
       <c r="K18">
+        <f>C18*2.5</f>
+        <v>22.5</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="M18">
         <v>12</v>
@@ -5012,41 +5017,44 @@
       <c r="A19">
         <v>421527</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="12" t="s">
         <v>35</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19">
         <v>10</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
       </c>
       <c r="H19">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I19">
         <v>15</v>
       </c>
       <c r="J19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19">
+        <f>C19*2.5</f>
+        <v>2.5</v>
+      </c>
+      <c r="L19">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M19">
         <v>12</v>
@@ -5088,12 +5096,12 @@
         <v>3</v>
       </c>
       <c r="K20">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="L20">
         <f t="shared" si="5"/>
         <v>7</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="4"/>
+        <v>13</v>
       </c>
       <c r="M20">
         <v>12</v>
@@ -5103,22 +5111,22 @@
       <c r="A21">
         <v>624690</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="12" t="s">
         <v>39</v>
       </c>
       <c r="C21">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>10</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G21">
         <v>12</v>
@@ -5131,16 +5139,16 @@
         <v>15</v>
       </c>
       <c r="J21">
-        <f t="shared" si="3"/>
-        <v>12</v>
+        <f ca="1">J21</f>
+        <v>0</v>
       </c>
       <c r="K21">
-        <f t="shared" si="4"/>
-        <v>18</v>
+        <f>C21*2.5</f>
+        <v>22.5</v>
       </c>
       <c r="L21">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f>_xlfn.RANK.EQ(K21,$K$2:$K$25)</f>
+        <v>2</v>
       </c>
       <c r="M21">
         <v>12</v>
@@ -5179,12 +5187,12 @@
         <v>0</v>
       </c>
       <c r="K22">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L22">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M22">
         <v>12</v>
@@ -5194,44 +5202,44 @@
       <c r="A23">
         <v>621172</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="12" t="s">
         <v>43</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E23">
         <v>10</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G23">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I23">
         <v>15</v>
       </c>
       <c r="J23">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K23">
+        <f>C23*2.5</f>
+        <v>20</v>
+      </c>
+      <c r="L23">
         <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="5"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="M23">
         <v>12</v>
@@ -5278,7 +5286,7 @@
       </c>
       <c r="L24">
         <f t="shared" ref="L24" si="11">_xlfn.RANK.EQ(K24,$K$2:$K$25)</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M24">
         <v>13</v>
@@ -5320,11 +5328,11 @@
         <v>14</v>
       </c>
       <c r="K25">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="L25">
         <f t="shared" si="4"/>
-        <v>24</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M25">
@@ -5341,7 +5349,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView zoomScale="92" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F25"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5435,12 +5443,12 @@
         <v>6</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K25" si="2">F3+J3</f>
+        <f t="shared" ref="K3:K8" si="2">F3+J3</f>
         <v>6</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L25" si="3">_xlfn.RANK.EQ(K3,$K$2:$K$25)</f>
-        <v>11</v>
+        <f t="shared" ref="L3:L8" si="3">_xlfn.RANK.EQ(K3,$K$2:$K$25)</f>
+        <v>14</v>
       </c>
       <c r="M3">
         <v>9</v>
@@ -5506,7 +5514,7 @@
       </c>
       <c r="L5">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M5">
         <v>9</v>
@@ -5539,7 +5547,7 @@
       </c>
       <c r="L6">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M6">
         <v>9</v>
@@ -5572,7 +5580,7 @@
       </c>
       <c r="L7">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="M7">
         <v>9</v>
@@ -5605,7 +5613,7 @@
       </c>
       <c r="L8">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M8">
         <v>9</v>
@@ -5619,26 +5627,26 @@
         <v>15</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E9">
         <v>20</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K9">
         <f t="shared" ref="K9:K25" si="4">F9+J9</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="L9">
         <f t="shared" ref="L9:L25" si="5">_xlfn.RANK.EQ(K9,$K$2:$K$25)</f>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="M9">
         <v>9</v>
@@ -5671,7 +5679,7 @@
       </c>
       <c r="L10">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M10">
         <v>9</v>
@@ -5704,7 +5712,7 @@
       </c>
       <c r="L11">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="M11">
         <v>9</v>
@@ -5737,7 +5745,7 @@
       </c>
       <c r="L12">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M12">
         <v>9</v>
@@ -5770,7 +5778,7 @@
       </c>
       <c r="L13">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M13">
         <v>9</v>
@@ -5784,26 +5792,26 @@
         <v>25</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E14">
         <v>20</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="K14">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="L14">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="M14">
         <v>9</v>
@@ -5836,7 +5844,7 @@
       </c>
       <c r="L15">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M15">
         <v>9</v>
@@ -5869,7 +5877,7 @@
       </c>
       <c r="L16">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M16">
         <v>9</v>
@@ -5902,7 +5910,7 @@
       </c>
       <c r="L17">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M17">
         <v>9</v>
@@ -5916,26 +5924,26 @@
         <v>33</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E18">
         <v>20</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="K18">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="L18">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="M18">
         <v>9</v>
@@ -5968,7 +5976,7 @@
       </c>
       <c r="L19">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="M19">
         <v>9</v>
@@ -6001,7 +6009,7 @@
       </c>
       <c r="L20">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M20">
         <v>9</v>
@@ -6067,7 +6075,7 @@
       </c>
       <c r="L22">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M22">
         <v>9</v>
@@ -6100,7 +6108,7 @@
       </c>
       <c r="L23">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M23">
         <v>9</v>
@@ -6182,7 +6190,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView zoomScale="96" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6247,7 +6255,7 @@
         <v>9</v>
       </c>
       <c r="L2">
-        <f>_xlfn.RANK.EQ(K2,$K$2:$K$25)</f>
+        <f t="shared" ref="L2:L8" si="0">_xlfn.RANK.EQ(K2,$K$2:$K$25)</f>
         <v>4</v>
       </c>
       <c r="M2">
@@ -6265,22 +6273,22 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D25" si="0">E3-C3</f>
+        <f t="shared" ref="D3:D25" si="1">E3-C3</f>
         <v>6</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F25" si="1">C3</f>
+        <f t="shared" ref="F3:F25" si="2">C3</f>
         <v>4</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K25" si="2">F3+J3</f>
+        <f t="shared" ref="K3:K25" si="3">F3+J3</f>
         <v>4</v>
       </c>
       <c r="L3">
-        <f>_xlfn.RANK.EQ(K3,$K$2:$K$25)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M3">
@@ -6298,22 +6306,22 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="K4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="L4">
-        <f>_xlfn.RANK.EQ(K4,$K$2:$K$25)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M4">
@@ -6328,26 +6336,26 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>10</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="K5">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="L5">
-        <f>_xlfn.RANK.EQ(K5,$K$2:$K$25)</f>
-        <v>17</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="M5">
         <v>6</v>
@@ -6364,22 +6372,22 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="K6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="L6">
-        <f>_xlfn.RANK.EQ(K6,$K$2:$K$25)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M6">
@@ -6397,23 +6405,23 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L7">
-        <f>_xlfn.RANK.EQ(K7,$K$2:$K$25)</f>
-        <v>17</v>
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="M7">
         <v>6</v>
@@ -6430,22 +6438,22 @@
         <v>9</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E8">
         <v>10</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="K8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="L8">
-        <f>_xlfn.RANK.EQ(K8,$K$2:$K$25)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="M8">
@@ -6463,22 +6471,22 @@
         <v>4</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L9">
-        <f t="shared" ref="L9:L18" si="3">_xlfn.RANK.EQ(K9,$K$2:$K$25)</f>
+        <f t="shared" ref="L9:L18" si="4">_xlfn.RANK.EQ(K9,$K$2:$K$25)</f>
         <v>12</v>
       </c>
       <c r="M9">
@@ -6496,23 +6504,23 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L10">
-        <f t="shared" si="3"/>
-        <v>17</v>
+        <f t="shared" si="4"/>
+        <v>19</v>
       </c>
       <c r="M10">
         <v>6</v>
@@ -6529,23 +6537,23 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="E11">
         <v>10</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L11">
-        <f t="shared" si="3"/>
-        <v>16</v>
+        <f t="shared" si="4"/>
+        <v>18</v>
       </c>
       <c r="M11">
         <v>6</v>
@@ -6562,23 +6570,23 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L12">
-        <f t="shared" si="3"/>
-        <v>17</v>
+        <f t="shared" si="4"/>
+        <v>19</v>
       </c>
       <c r="M12">
         <v>6</v>
@@ -6595,22 +6603,22 @@
         <v>6</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E13">
         <v>10</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="K13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="L13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="M13">
@@ -6628,22 +6636,22 @@
         <v>10</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E14">
         <v>10</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="K14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="L14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M14">
@@ -6661,23 +6669,23 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="E15">
         <v>10</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L15">
-        <f t="shared" si="3"/>
-        <v>17</v>
+        <f t="shared" si="4"/>
+        <v>19</v>
       </c>
       <c r="M15">
         <v>6</v>
@@ -6694,23 +6702,23 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="E16">
         <v>10</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L16">
-        <f t="shared" si="3"/>
-        <v>17</v>
+        <f t="shared" si="4"/>
+        <v>19</v>
       </c>
       <c r="M16">
         <v>6</v>
@@ -6727,23 +6735,23 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="E17">
         <v>10</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L17">
-        <f t="shared" si="3"/>
-        <v>17</v>
+        <f t="shared" si="4"/>
+        <v>19</v>
       </c>
       <c r="M17">
         <v>6</v>
@@ -6760,22 +6768,22 @@
         <v>5</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="E18">
         <v>10</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="K18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="L18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="M18">
@@ -6790,26 +6798,26 @@
         <v>35</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="E19">
         <v>10</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="K19">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="L19">
-        <f>_xlfn.RANK.EQ(K19,$K$2:$K$25)</f>
-        <v>15</v>
+        <f t="shared" ref="L19:L25" si="5">_xlfn.RANK.EQ(K19,$K$2:$K$25)</f>
+        <v>12</v>
       </c>
       <c r="M19">
         <v>6</v>
@@ -6823,26 +6831,26 @@
         <v>37</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="E20">
         <v>10</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="K20">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>3</v>
       </c>
       <c r="L20">
-        <f>_xlfn.RANK.EQ(K20,$K$2:$K$25)</f>
-        <v>17</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
       <c r="M20">
         <v>6</v>
@@ -6859,22 +6867,22 @@
         <v>10</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E21">
         <v>10</v>
       </c>
       <c r="F21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="K21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="L21">
-        <f>_xlfn.RANK.EQ(K21,$K$2:$K$25)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M21">
@@ -6892,22 +6900,22 @@
         <v>6</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E22">
         <v>10</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="K22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="L22">
-        <f>_xlfn.RANK.EQ(K22,$K$2:$K$25)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="M22">
@@ -6925,23 +6933,23 @@
         <v>3</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="E23">
         <v>10</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="L23">
-        <f>_xlfn.RANK.EQ(K23,$K$2:$K$25)</f>
-        <v>14</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
       <c r="M23">
         <v>6</v>
@@ -6958,22 +6966,22 @@
         <v>6</v>
       </c>
       <c r="D24">
-        <f t="shared" ref="D24" si="4">E24-C24</f>
+        <f t="shared" ref="D24" si="6">E24-C24</f>
         <v>4</v>
       </c>
       <c r="E24">
         <v>10</v>
       </c>
       <c r="F24">
-        <f t="shared" ref="F24" si="5">C24</f>
+        <f t="shared" ref="F24" si="7">C24</f>
         <v>6</v>
       </c>
       <c r="K24">
-        <f t="shared" ref="K24" si="6">F24+J24</f>
+        <f t="shared" ref="K24" si="8">F24+J24</f>
         <v>6</v>
       </c>
       <c r="L24">
-        <f>_xlfn.RANK.EQ(K24,$K$2:$K$25)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="M24">
@@ -6991,22 +6999,22 @@
         <v>10</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E25">
         <v>10</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="K25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="L25">
-        <f>_xlfn.RANK.EQ(K25,$K$2:$K$25)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M25">
@@ -7027,7 +7035,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7107,26 +7115,26 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D25" si="0">E3-C3</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F25" si="1">C3</f>
-        <v>0</v>
+        <f t="shared" ref="F3:F6" si="1">C3</f>
+        <v>2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K25" si="2">F3+J3</f>
-        <v>0</v>
+        <f t="shared" ref="K3:K6" si="2">F3+J3</f>
+        <v>2</v>
       </c>
       <c r="L3">
         <f>_xlfn.RANK.EQ(K3,$K$2:$K$25)</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M3">
         <v>6</v>
@@ -7173,26 +7181,26 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>10</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <f>_xlfn.RANK.EQ(K5,$K$2:$K$25)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M5">
         <v>6</v>
@@ -7225,7 +7233,7 @@
       </c>
       <c r="L6">
         <f t="shared" ref="L6:L25" si="3">_xlfn.RANK.EQ(K6,$K$2:$K$25)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M6">
         <v>6</v>
@@ -7258,7 +7266,7 @@
       </c>
       <c r="L7">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M7">
         <v>6</v>
@@ -7272,26 +7280,26 @@
         <v>13</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E8">
         <v>10</v>
       </c>
       <c r="F8">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K8">
         <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="3"/>
         <v>3</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="3"/>
-        <v>8</v>
       </c>
       <c r="M8">
         <v>6</v>
@@ -7305,26 +7313,26 @@
         <v>15</v>
       </c>
       <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
         <v>4</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>6</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
       <c r="F9">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K9">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L9">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M9">
         <v>6</v>
@@ -7357,7 +7365,7 @@
       </c>
       <c r="L10">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M10">
         <v>6</v>
@@ -7390,7 +7398,7 @@
       </c>
       <c r="L11">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M11">
         <v>6</v>
@@ -7423,7 +7431,7 @@
       </c>
       <c r="L12">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M12">
         <v>6</v>
@@ -7456,7 +7464,7 @@
       </c>
       <c r="L13">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="M13">
         <v>6</v>
@@ -7522,7 +7530,7 @@
       </c>
       <c r="L15">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M15">
         <v>6</v>
@@ -7555,7 +7563,7 @@
       </c>
       <c r="L16">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M16">
         <v>6</v>
@@ -7588,7 +7596,7 @@
       </c>
       <c r="L17">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M17">
         <v>6</v>
@@ -7602,26 +7610,26 @@
         <v>33</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E18">
         <v>10</v>
       </c>
       <c r="F18">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K18">
         <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="3"/>
         <v>3</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="3"/>
-        <v>8</v>
       </c>
       <c r="M18">
         <v>6</v>
@@ -7635,26 +7643,26 @@
         <v>35</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19">
         <v>10</v>
       </c>
       <c r="F19">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K19">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L19">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M19">
         <v>6</v>
@@ -7668,26 +7676,26 @@
         <v>37</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E20">
         <v>10</v>
       </c>
       <c r="F20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L20">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="M20">
         <v>6</v>
@@ -7720,7 +7728,7 @@
       </c>
       <c r="L21">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M21">
         <v>6</v>
@@ -7753,7 +7761,7 @@
       </c>
       <c r="L22">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="M22">
         <v>6</v>
@@ -7767,26 +7775,26 @@
         <v>43</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E23">
         <v>10</v>
       </c>
       <c r="F23">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K23">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L23">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="M23">
         <v>6</v>
@@ -7819,7 +7827,7 @@
       </c>
       <c r="L24">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="M24">
         <v>6</v>
@@ -7872,7 +7880,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7941,7 +7949,7 @@
       </c>
       <c r="L2" s="11">
         <f>_xlfn.RANK.EQ(K2,$K$2:$K$25)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M2" s="10">
         <v>30</v>
@@ -7956,18 +7964,18 @@
       </c>
       <c r="C3" s="10">
         <f>'English Quiz 1'!K3/3+'English Quiz 2'!F3/2+'English Quiz 3'!K3/2.5+'English Quiz 4'!K3+'English Quiz 5'!K3</f>
-        <v>11.333333333333334</v>
+        <v>15.333333333333334</v>
       </c>
       <c r="D3" s="10">
         <f t="shared" ref="D3:D25" si="0">E3-C3</f>
-        <v>38.666666666666664</v>
+        <v>34.666666666666664</v>
       </c>
       <c r="E3" s="10">
         <v>50</v>
       </c>
       <c r="F3" s="10">
         <f t="shared" ref="F3:F25" si="1">C3</f>
-        <v>11.333333333333334</v>
+        <v>15.333333333333334</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
@@ -7975,11 +7983,11 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10">
         <f t="shared" ref="K3:K25" si="2">F3+J3</f>
-        <v>11.333333333333334</v>
+        <v>15.333333333333334</v>
       </c>
       <c r="L3" s="11">
         <f>_xlfn.RANK.EQ(K3,$K$2:$K$25)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M3" s="10">
         <v>30</v>
@@ -7994,18 +8002,18 @@
       </c>
       <c r="C4" s="10">
         <f>'English Quiz 1'!K4/3+'English Quiz 2'!F4/2+'English Quiz 3'!K4/2.5+'English Quiz 4'!K4+'English Quiz 5'!K4</f>
-        <v>30.4</v>
+        <v>36</v>
       </c>
       <c r="D4" s="10">
         <f t="shared" si="0"/>
-        <v>19.600000000000001</v>
+        <v>14</v>
       </c>
       <c r="E4" s="10">
         <v>50</v>
       </c>
       <c r="F4" s="10">
         <f t="shared" si="1"/>
-        <v>30.4</v>
+        <v>36</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
@@ -8013,11 +8021,11 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10">
         <f t="shared" si="2"/>
-        <v>30.4</v>
+        <v>36</v>
       </c>
       <c r="L4" s="11">
         <f>_xlfn.RANK.EQ(K4,$K$2:$K$25)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M4" s="10">
         <v>30</v>
@@ -8032,18 +8040,18 @@
       </c>
       <c r="C5" s="10">
         <f>'English Quiz 1'!K5/3+'English Quiz 2'!F5/2+'English Quiz 3'!K5/2.5+'English Quiz 4'!K5+'English Quiz 5'!K5</f>
-        <v>13.233333333333333</v>
+        <v>18.233333333333334</v>
       </c>
       <c r="D5" s="10">
         <f t="shared" si="0"/>
-        <v>36.766666666666666</v>
+        <v>31.766666666666666</v>
       </c>
       <c r="E5" s="10">
         <v>50</v>
       </c>
       <c r="F5" s="10">
         <f t="shared" si="1"/>
-        <v>13.233333333333333</v>
+        <v>18.233333333333334</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
@@ -8051,11 +8059,11 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10">
         <f t="shared" si="2"/>
-        <v>13.233333333333333</v>
+        <v>18.233333333333334</v>
       </c>
       <c r="L5" s="11">
         <f>_xlfn.RANK.EQ(K5,$K$2:$K$25)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M5" s="10">
         <v>30</v>
@@ -8093,7 +8101,7 @@
       </c>
       <c r="L6" s="11">
         <f t="shared" ref="L6:L25" si="3">_xlfn.RANK.EQ(K6,$K$2:$K$25)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M6" s="10">
         <v>30</v>
@@ -8146,18 +8154,18 @@
       </c>
       <c r="C8" s="10">
         <f>'English Quiz 1'!K8/3+'English Quiz 2'!F8/2+'English Quiz 3'!K8/2.5+'English Quiz 4'!K8+'English Quiz 5'!K8</f>
-        <v>30.8</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="D8" s="10">
         <f t="shared" si="0"/>
-        <v>19.2</v>
+        <v>16.200000000000003</v>
       </c>
       <c r="E8" s="10">
         <v>50</v>
       </c>
       <c r="F8" s="10">
         <f t="shared" si="1"/>
-        <v>30.8</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -8165,11 +8173,11 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10">
         <f t="shared" si="2"/>
-        <v>30.8</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="L8" s="11">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M8" s="10">
         <v>30</v>
@@ -8184,18 +8192,18 @@
       </c>
       <c r="C9" s="10">
         <f>'English Quiz 1'!K9/3+'English Quiz 2'!F9/2+'English Quiz 3'!K9/2.5+'English Quiz 4'!K9+'English Quiz 5'!K9</f>
-        <v>8.9</v>
+        <v>22.166666666666664</v>
       </c>
       <c r="D9" s="10">
         <f t="shared" si="0"/>
-        <v>41.1</v>
+        <v>27.833333333333336</v>
       </c>
       <c r="E9" s="10">
         <v>50</v>
       </c>
       <c r="F9" s="10">
         <f t="shared" si="1"/>
-        <v>8.9</v>
+        <v>22.166666666666664</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -8203,11 +8211,11 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10">
         <f t="shared" si="2"/>
-        <v>8.9</v>
+        <v>22.166666666666664</v>
       </c>
       <c r="L9" s="11">
         <f t="shared" si="3"/>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="M9" s="10">
         <v>30</v>
@@ -8260,18 +8268,18 @@
       </c>
       <c r="C11" s="10">
         <f>'English Quiz 1'!K11/3+'English Quiz 2'!F11/2+'English Quiz 3'!K11/2.5+'English Quiz 4'!K11+'English Quiz 5'!K11</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D11" s="10">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E11" s="10">
         <v>50</v>
       </c>
       <c r="F11" s="10">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -8279,11 +8287,11 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="L11" s="11">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M11" s="10">
         <v>30</v>
@@ -8359,7 +8367,7 @@
       </c>
       <c r="L13" s="11">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="M13" s="10">
         <v>30</v>
@@ -8374,18 +8382,18 @@
       </c>
       <c r="C14" s="10">
         <f>'English Quiz 1'!K14/3+'English Quiz 2'!F14/2+'English Quiz 3'!K14/2.5+'English Quiz 4'!K14+'English Quiz 5'!K14</f>
-        <v>32.1</v>
+        <v>44</v>
       </c>
       <c r="D14" s="10">
         <f t="shared" si="0"/>
-        <v>17.899999999999999</v>
+        <v>6</v>
       </c>
       <c r="E14" s="10">
         <v>50</v>
       </c>
       <c r="F14" s="10">
         <f t="shared" si="1"/>
-        <v>32.1</v>
+        <v>44</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -8393,11 +8401,11 @@
       <c r="J14" s="10"/>
       <c r="K14" s="10">
         <f t="shared" si="2"/>
-        <v>32.1</v>
+        <v>44</v>
       </c>
       <c r="L14" s="11">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M14" s="10">
         <v>30</v>
@@ -8526,18 +8534,18 @@
       </c>
       <c r="C18" s="10">
         <f>'English Quiz 1'!K18/3+'English Quiz 2'!F18/2+'English Quiz 3'!K18/2.5+'English Quiz 4'!K18+'English Quiz 5'!K18</f>
-        <v>8.5</v>
+        <v>36</v>
       </c>
       <c r="D18" s="10">
         <f t="shared" si="0"/>
-        <v>41.5</v>
+        <v>14</v>
       </c>
       <c r="E18" s="10">
         <v>50</v>
       </c>
       <c r="F18" s="10">
         <f t="shared" si="1"/>
-        <v>8.5</v>
+        <v>36</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
@@ -8545,11 +8553,11 @@
       <c r="J18" s="10"/>
       <c r="K18" s="10">
         <f t="shared" si="2"/>
-        <v>8.5</v>
+        <v>36</v>
       </c>
       <c r="L18" s="11">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="M18" s="10">
         <v>30</v>
@@ -8564,18 +8572,18 @@
       </c>
       <c r="C19" s="10">
         <f>'English Quiz 1'!K19/3+'English Quiz 2'!F19/2+'English Quiz 3'!K19/2.5+'English Quiz 4'!K19+'English Quiz 5'!K19</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D19" s="10">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E19" s="10">
         <v>50</v>
       </c>
       <c r="F19" s="10">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
@@ -8583,11 +8591,11 @@
       <c r="J19" s="10"/>
       <c r="K19" s="10">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="L19" s="11">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M19" s="10">
         <v>30</v>
@@ -8602,18 +8610,18 @@
       </c>
       <c r="C20" s="10">
         <f>'English Quiz 1'!K20/3+'English Quiz 2'!F20/2+'English Quiz 3'!K20/2.5+'English Quiz 4'!K20+'English Quiz 5'!K20</f>
-        <v>13.8</v>
+        <v>19.8</v>
       </c>
       <c r="D20" s="10">
         <f t="shared" si="0"/>
-        <v>36.200000000000003</v>
+        <v>30.2</v>
       </c>
       <c r="E20" s="10">
         <v>50</v>
       </c>
       <c r="F20" s="10">
         <f t="shared" si="1"/>
-        <v>13.8</v>
+        <v>19.8</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
@@ -8621,11 +8629,11 @@
       <c r="J20" s="10"/>
       <c r="K20" s="10">
         <f t="shared" si="2"/>
-        <v>13.8</v>
+        <v>19.8</v>
       </c>
       <c r="L20" s="11">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M20" s="10">
         <v>30</v>
@@ -8640,18 +8648,18 @@
       </c>
       <c r="C21" s="10">
         <f>'English Quiz 1'!K21/3+'English Quiz 2'!F21/2+'English Quiz 3'!K21/2.5+'English Quiz 4'!K21+'English Quiz 5'!K21</f>
-        <v>40.700000000000003</v>
+        <v>42.5</v>
       </c>
       <c r="D21" s="10">
         <f t="shared" si="0"/>
-        <v>9.2999999999999972</v>
+        <v>7.5</v>
       </c>
       <c r="E21" s="10">
         <v>50</v>
       </c>
       <c r="F21" s="10">
         <f t="shared" si="1"/>
-        <v>40.700000000000003</v>
+        <v>42.5</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
@@ -8659,7 +8667,7 @@
       <c r="J21" s="10"/>
       <c r="K21" s="10">
         <f t="shared" si="2"/>
-        <v>40.700000000000003</v>
+        <v>42.5</v>
       </c>
       <c r="L21" s="11">
         <f t="shared" si="3"/>
@@ -8701,7 +8709,7 @@
       </c>
       <c r="L22" s="11">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="M22" s="10">
         <v>30</v>
@@ -8716,18 +8724,18 @@
       </c>
       <c r="C23" s="10">
         <f>'English Quiz 1'!K23/3+'English Quiz 2'!F23/2+'English Quiz 3'!K23/2.5+'English Quiz 4'!K23+'English Quiz 5'!K23</f>
-        <v>14.6</v>
+        <v>24</v>
       </c>
       <c r="D23" s="10">
         <f t="shared" si="0"/>
-        <v>35.4</v>
+        <v>26</v>
       </c>
       <c r="E23" s="10">
         <v>50</v>
       </c>
       <c r="F23" s="10">
         <f t="shared" si="1"/>
-        <v>14.6</v>
+        <v>24</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
@@ -8735,11 +8743,11 @@
       <c r="J23" s="10"/>
       <c r="K23" s="10">
         <f t="shared" si="2"/>
-        <v>14.6</v>
+        <v>24</v>
       </c>
       <c r="L23" s="11">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M23" s="10">
         <v>30</v>
@@ -8777,7 +8785,7 @@
       </c>
       <c r="L24" s="11">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="M24" s="10">
         <v>30</v>
@@ -8824,7 +8832,7 @@
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K28" s="10">
         <f>AVERAGE(K2:K25)+_xlfn.STDEV.P(K2:K25)</f>
-        <v>30.420217565829539</v>
+        <v>35.264169750881102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add essay marks display for full tests and auto-detect Excel files
</commit_message>
<xml_diff>
--- a/Results/Simple Test Data.xlsx
+++ b/Results/Simple Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VH Website\vh-website\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F88173B-B7D5-4373-B916-DAD20A19BB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339036D4-677E-4084-BA6A-016113112C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
@@ -1578,7 +1578,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2345,7 +2345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DAE4A7-33AC-4249-9023-01333106F7E9}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A23" sqref="A23:B24"/>
     </sheetView>
   </sheetViews>
@@ -4424,7 +4424,7 @@
         <v>4</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K3:K25" si="5">F5+J5</f>
+        <f t="shared" ref="K5:K25" si="5">F5+J5</f>
         <v>6</v>
       </c>
       <c r="L5">
@@ -7879,7 +7879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B3BE9F-BEF9-4B86-BC39-943270B2720E}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>